<commit_message>
Added self-assessment questions to all chapter 12 lessons.
</commit_message>
<xml_diff>
--- a/scratch_files/perspective_calculations.xlsx
+++ b/scratch_files/perspective_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bettybrown/Documents/Runestone/learnwebgl2/scratch_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{D311F9ED-5A65-DF46-ADF0-FDE87E6BE90E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{E5F8B898-4528-D244-9A08-F14DE82AD039}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="30160" windowHeight="15100" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3286,7 +3286,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
                 <c:pt idx="0">
-                  <c:v>1.1408696209969094E-10</c:v>
+                  <c:v>0.96078433865469903</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-2.9354361252842409E-7</c:v>
@@ -6206,25 +6206,25 @@
     <row r="55" spans="1:9" x14ac:dyDescent="0.15">
       <c r="I55">
         <f ca="1">RANDBETWEEN(2,13)</f>
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.15">
       <c r="I56">
         <f ca="1">RANDBETWEEN(20,50)</f>
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.15">
       <c r="I59" s="2">
         <f ca="1">-(2*I55*I56)/(I55-I56)</f>
-        <v>22.90909090909091</v>
+        <v>4.2051282051282053</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.15">
       <c r="I60" s="3">
         <f ca="1">(2*I55*I56)/(I56-I55)</f>
-        <v>22.90909090909091</v>
+        <v>4.2051282051282053</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.15">
@@ -6254,8 +6254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6851927-19FC-B448-8F8E-C40A5DCBA296}">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5:H54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6362,8 +6362,8 @@
         <v>1.6E-7</v>
       </c>
       <c r="H5">
-        <f>constant1/(B5+(1/2^32)-constant2) + A5</f>
-        <v>1.1408696209969094E-10</v>
+        <f>constant1/(C5+(1/2^32)-constant2) + A5</f>
+        <v>0.96078433865469903</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.15">
@@ -7986,25 +7986,25 @@
     <row r="58" spans="1:9" x14ac:dyDescent="0.15">
       <c r="I58">
         <f ca="1">RANDBETWEEN(2,13)</f>
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.15">
       <c r="I59">
         <f ca="1">RANDBETWEEN(20,50)</f>
-        <v>25</v>
+        <v>36</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.15">
       <c r="I62" s="2">
         <f ca="1">-(2*I58*I59)/(I58-I59)</f>
-        <v>46.153846153846153</v>
+        <v>14.4</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.15">
       <c r="I63" s="3">
         <f ca="1">(2*I58*I59)/(I59-I58)</f>
-        <v>46.153846153846153</v>
+        <v>14.4</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.15">

</xml_diff>